<commit_message>
Change-Id: I1d60b51b6d317352ad65306aafc81a1bd6534382 Signed-off-by: Trance <Trance@Trance-pc>
</commit_message>
<xml_diff>
--- a/cool/first/res/Control group 2.xlsx
+++ b/cool/first/res/Control group 2.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId5"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId6"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="57">
   <si>
     <t>FII G20210A</t>
   </si>
@@ -23,7 +26,7 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -40,7 +43,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="11"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -207,22 +210,17 @@
   <si>
     <t>con-30</t>
   </si>
+  <si>
+    <t>ФИО</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -232,12 +230,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -291,66 +284,110 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -476,7 +513,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -485,7 +522,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -494,7 +531,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -558,8 +595,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -567,7 +604,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -575,7 +612,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -594,7 +631,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -602,7 +639,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -630,7 +667,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +693,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -682,7 +719,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +745,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +771,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +797,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +823,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +849,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -838,7 +875,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -851,9 +888,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -870,7 +913,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -889,7 +932,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +958,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +984,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +1010,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +1036,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1062,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1088,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1114,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1140,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1166,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1136,9 +1179,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1152,7 +1201,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1171,7 +1220,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1250,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1276,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1302,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1328,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1354,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1380,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1406,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1432,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1409,7 +1458,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1422,1312 +1471,1322 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.17188" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.17188" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.17188" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6719" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1719" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.3516" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.17188" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6719" style="1" customWidth="1"/>
-    <col min="16" max="256" width="8.85156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="1" customWidth="1"/>
+    <col min="16" max="256" width="8.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+    <row r="1" spans="1:15" ht="30" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s" s="3">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s" s="3">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s" s="3">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s" s="3">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s" s="3">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s" s="3">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="4">
+    <row r="2" spans="1:15" ht="15" customHeight="1">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s" s="4">
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s" s="4">
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s" s="4">
+      <c r="H2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s" s="5">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L2" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s" s="4">
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s" s="4">
+      <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O2" t="s" s="4">
+      <c r="O2" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:15" ht="15" customHeight="1">
+      <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s" s="4">
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="4">
+      <c r="E3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s" s="5">
+      <c r="G3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s" s="4">
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s" s="5">
+      <c r="J3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K3" t="s" s="6">
+      <c r="K3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s" s="4">
+      <c r="L3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N3" t="s" s="4">
+      <c r="N3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="4">
+      <c r="O3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" customHeight="1">
+      <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s" s="5">
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" t="s" s="5">
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s" s="4">
+      <c r="I4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s" s="5">
+      <c r="J4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s" s="6">
+      <c r="K4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M4" t="s" s="4">
+      <c r="M4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" t="s" s="4">
+      <c r="N4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="4">
+      <c r="O4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1">
+      <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s" s="5">
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s" s="5">
+      <c r="H5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s" s="4">
+      <c r="I5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s" s="5">
+      <c r="J5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s" s="4">
+      <c r="K5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N5" t="s" s="4">
+      <c r="N5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O5" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="4">
+      <c r="O5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" customHeight="1">
+      <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s" s="5">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I6" t="s" s="4">
+      <c r="H6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J6" t="s" s="5">
+      <c r="J6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K6" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L6" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M6" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s" s="4">
+      <c r="K6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O6" t="s" s="4">
+      <c r="O6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="4">
+    <row r="7" spans="1:15" ht="15" customHeight="1">
+      <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s" s="5">
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s" s="4">
+      <c r="H7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s" s="5">
+      <c r="J7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K7" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L7" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M7" t="s" s="4">
+      <c r="K7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N7" t="s" s="4">
+      <c r="N7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O7" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1">
-      <c r="A8" t="s" s="4">
+      <c r="O7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" customHeight="1">
+      <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s" s="4">
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s" s="5">
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I8" t="s" s="4">
+      <c r="H8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J8" t="s" s="5">
+      <c r="J8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K8" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L8" t="s" s="6">
+      <c r="K8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M8" t="s" s="4">
+      <c r="M8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N8" t="s" s="4">
+      <c r="N8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O8" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1">
-      <c r="A9" t="s" s="4">
+      <c r="O8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1">
+      <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s" s="4">
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G9" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s" s="4">
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J9" t="s" s="5">
+      <c r="J9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K9" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s" s="4">
+      <c r="K9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N9" t="s" s="4">
+      <c r="N9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O9" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1">
-      <c r="A10" t="s" s="4">
+      <c r="O9" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" customHeight="1">
+      <c r="A10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s" s="4">
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F10" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s" s="5">
+      <c r="E10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s" s="4">
+      <c r="H10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J10" t="s" s="5">
+      <c r="J10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="K10" t="s" s="6">
+      <c r="K10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L10" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M10" t="s" s="4">
+      <c r="L10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N10" t="s" s="4">
+      <c r="N10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O10" t="s" s="4">
+      <c r="O10" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1">
-      <c r="A11" t="s" s="4">
+    <row r="11" spans="1:15" ht="15" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s" s="4">
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E11" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s" s="5">
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s" s="5">
+      <c r="H11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I11" t="s" s="4">
+      <c r="I11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J11" t="s" s="5">
+      <c r="J11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K11" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L11" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M11" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="N11" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="O11" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1">
-      <c r="A12" t="s" s="4">
+      <c r="K11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" customHeight="1">
+      <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B12" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F12" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s" s="5">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H12" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s" s="4">
+      <c r="H12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J12" t="s" s="5">
+      <c r="J12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K12" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L12" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M12" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="N12" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="O12" t="s" s="4">
+      <c r="K12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1">
-      <c r="A13" t="s" s="4">
+    <row r="13" spans="1:15" ht="15" customHeight="1">
+      <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F13" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G13" t="s" s="5">
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H13" t="s" s="5">
+      <c r="H13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I13" t="s" s="4">
+      <c r="I13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J13" t="s" s="4">
+      <c r="J13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K13" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L13" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M13" t="s" s="4">
+      <c r="K13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N13" t="s" s="4">
+      <c r="N13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O13" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1">
-      <c r="A14" t="s" s="4">
+      <c r="O13" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D14" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E14" t="s" s="4">
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H14" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s" s="4">
+      <c r="F14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J14" t="s" s="4">
+      <c r="J14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K14" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L14" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M14" t="s" s="4">
+      <c r="K14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N14" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="O14" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1">
-      <c r="A15" t="s" s="4">
+      <c r="N14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s" s="4">
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J15" t="s" s="4">
+      <c r="J15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K15" t="s" s="6">
+      <c r="K15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L15" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M15" t="s" s="4">
+      <c r="L15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N15" t="s" s="4">
+      <c r="N15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O15" t="s" s="4">
+      <c r="O15" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1">
-      <c r="A16" t="s" s="4">
+    <row r="16" spans="1:15" ht="15" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G16" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H16" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s" s="4">
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J16" t="s" s="4">
+      <c r="J16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K16" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L16" t="s" s="6">
+      <c r="K16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M16" t="s" s="4">
+      <c r="M16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N16" t="s" s="4">
+      <c r="N16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O16" t="s" s="4">
+      <c r="O16" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1">
-      <c r="A17" t="s" s="4">
+    <row r="17" spans="1:15" ht="15" customHeight="1">
+      <c r="A17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B17" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s" s="4">
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="s" s="4">
+      <c r="E17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F17" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s" s="5">
+      <c r="F17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H17" t="s" s="5">
+      <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I17" t="s" s="4">
+      <c r="I17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J17" t="s" s="4">
+      <c r="J17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K17" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L17" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M17" t="s" s="4">
+      <c r="K17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N17" t="s" s="4">
+      <c r="N17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O17" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1">
-      <c r="A18" t="s" s="4">
+      <c r="O17" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" customHeight="1">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F18" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G18" t="s" s="5">
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H18" t="s" s="5">
+      <c r="H18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I18" t="s" s="4">
+      <c r="I18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J18" t="s" s="4">
+      <c r="J18" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K18" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L18" t="s" s="6">
+      <c r="K18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M18" t="s" s="4">
+      <c r="M18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N18" t="s" s="4">
+      <c r="N18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O18" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1">
-      <c r="A19" t="s" s="4">
+      <c r="O18" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" customHeight="1">
+      <c r="A19" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D19" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="F19" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G19" t="s" s="5">
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H19" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I19" t="s" s="4">
+      <c r="H19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J19" t="s" s="4">
+      <c r="J19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K19" t="s" s="6">
+      <c r="K19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L19" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M19" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="N19" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="O19" t="s" s="4">
+      <c r="L19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O19" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1">
-      <c r="A20" t="s" s="4">
+    <row r="20" spans="1:15" ht="15" customHeight="1">
+      <c r="A20" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F20" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G20" t="s" s="5">
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H20" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I20" t="s" s="4">
+      <c r="H20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J20" t="s" s="4">
+      <c r="J20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K20" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L20" t="s" s="6">
+      <c r="K20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M20" t="s" s="4">
+      <c r="M20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N20" t="s" s="4">
+      <c r="N20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O20" t="s" s="4">
+      <c r="O20" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1">
-      <c r="A21" t="s" s="4">
+    <row r="21" spans="1:15" ht="15" customHeight="1">
+      <c r="A21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F21" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G21" t="s" s="5">
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H21" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s" s="4">
+      <c r="H21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J21" t="s" s="4">
+      <c r="J21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K21" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L21" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M21" t="s" s="4">
+      <c r="K21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N21" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="O21" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1">
-      <c r="A22" t="s" s="4">
+      <c r="N21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" customHeight="1">
+      <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B22" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D22" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F22" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s" s="5">
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H22" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I22" t="s" s="4">
+      <c r="H22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J22" t="s" s="4">
+      <c r="J22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K22" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L22" t="s" s="6">
+      <c r="K22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M22" t="s" s="4">
+      <c r="M22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N22" t="s" s="4">
+      <c r="N22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O22" t="s" s="4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1">
-      <c r="A23" t="s" s="4">
+      <c r="O22" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" customHeight="1">
+      <c r="A23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B23" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D23" t="s" s="4">
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s" s="4">
+      <c r="E23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G23" t="s" s="5">
+      <c r="G23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H23" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I23" t="s" s="4">
+      <c r="H23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J23" t="s" s="4">
+      <c r="J23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K23" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L23" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M23" t="s" s="4">
+      <c r="K23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N23" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="O23" t="s" s="4">
+      <c r="N23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O23" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1">
-      <c r="A24" t="s" s="4">
+    <row r="24" spans="1:15" ht="15" customHeight="1">
+      <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B24" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F24" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G24" t="s" s="5">
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H24" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I24" t="s" s="4">
+      <c r="H24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J24" t="s" s="4">
+      <c r="J24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K24" t="s" s="6">
+      <c r="K24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L24" t="s" s="6">
+      <c r="L24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M24" t="s" s="4">
+      <c r="M24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N24" t="s" s="4">
+      <c r="N24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O24" t="s" s="4">
+      <c r="O24" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1">
-      <c r="A25" t="s" s="4">
+    <row r="25" spans="1:15" ht="15" customHeight="1">
+      <c r="A25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D25" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="G25" t="s" s="5">
-        <v>15</v>
-      </c>
-      <c r="H25" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="I25" t="s" s="4">
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J25" t="s" s="4">
+      <c r="J25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K25" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="L25" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="M25" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="N25" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="O25" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1">
-      <c r="A26" t="s" s="4">
+      <c r="K25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C26" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="D26" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F26" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G26" t="s" s="5">
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H26" t="s" s="5">
+      <c r="H26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I26" t="s" s="4">
+      <c r="I26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J26" t="s" s="4">
+      <c r="J26" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K26" t="s" s="6">
+      <c r="K26" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L26" t="s" s="6">
+      <c r="L26" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M26" t="s" s="4">
+      <c r="M26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N26" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="O26" t="s" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1">
-      <c r="A27" t="s" s="4">
+      <c r="N26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" customHeight="1">
+      <c r="A27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s" s="4">
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D27" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="F27" t="s" s="4">
-        <v>17</v>
-      </c>
-      <c r="G27" t="s" s="5">
+      <c r="D27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H27" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="I27" t="s" s="4">
+      <c r="H27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J27" t="s" s="4">
+      <c r="J27" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K27" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="L27" t="s" s="6">
+      <c r="K27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M27" t="s" s="4">
+      <c r="M27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N27" t="s" s="4">
+      <c r="N27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O27" t="s" s="4">
+      <c r="O27" s="4" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2735,85 +2794,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="7" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="7" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="7" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="7" customWidth="1"/>
+    <col min="1" max="256" width="8.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2822,7 +2876,7 @@
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2830,85 +2884,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="9" customWidth="1"/>
-    <col min="2" max="2" width="8.85156" style="9" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="9" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="9" customWidth="1"/>
-    <col min="6" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="256" width="8.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
+    <row r="1" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="17.100000000000001" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -2917,7 +2966,7 @@
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Change-Id: I142a6b65a0e409927b6270b0eb0352ecae8d9381 Signed-off-by: Trance <Trance@Trance-pc>
</commit_message>
<xml_diff>
--- a/cool/first/res/Control group 2.xlsx
+++ b/cool/first/res/Control group 2.xlsx
@@ -82,9 +82,6 @@
     <t>ADRB2</t>
   </si>
   <si>
-    <t>IL-6             -174 G/С</t>
-  </si>
-  <si>
     <t>con-01</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>ФИО</t>
+  </si>
+  <si>
+    <t>IL-6 -174 G/С</t>
   </si>
 </sst>
 </file>
@@ -1493,7 +1493,7 @@
   <dimension ref="A1:IV27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -1517,7 +1517,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1559,1229 +1559,1229 @@
         <v>12</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="N2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="M4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="5" t="s">
+      <c r="N5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="O5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="K6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="K7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="J8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="E10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="K10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="J11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="J12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N16" s="4" t="s">
+      <c r="O16" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O16" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1">
       <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="J17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="5" t="s">
+      <c r="I18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N18" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="K19" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="K20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="E23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K24" s="6" t="s">
+      <c r="L24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="J25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="I26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="5" t="s">
+      <c r="L26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="N26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="D27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="N27" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>